<commit_message>
Melhorias no texto da Introdução do TCC
</commit_message>
<xml_diff>
--- a/mono/Fichamento - Referencial Teórico.xlsx
+++ b/mono/Fichamento - Referencial Teórico.xlsx
@@ -136,9 +136,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -160,6 +157,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -180,15 +180,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>8039100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -212,7 +212,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="1352550"/>
+          <a:off x="133350" y="1438275"/>
           <a:ext cx="8810625" cy="5429250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -235,15 +235,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>8029575</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -267,7 +267,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="7096125"/>
+          <a:off x="85725" y="7143750"/>
           <a:ext cx="8848725" cy="5429250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -579,81 +579,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="115.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="123.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+      <c r="A35" s="6">
         <v>3</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="10"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="9"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="9"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+      <c r="A65" s="11">
         <v>4</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="11" t="s">
+      <c r="A66" s="11"/>
+      <c r="B66" s="10" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>